<commit_message>
orthography and list work update
</commit_message>
<xml_diff>
--- a/OrthographyProfiles/OrthographyProfiles.xlsx
+++ b/OrthographyProfiles/OrthographyProfiles.xlsx
@@ -8,44 +8,45 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/auderset/Documents/GitHub/mixteca/OrthographyProfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6551BBF5-3C75-7944-A530-74F54367986B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF2F082-C502-D24C-9191-88A4D889F773}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="460" windowWidth="21600" windowHeight="16380" tabRatio="500" firstSheet="19" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5120" yWindow="6360" windowWidth="21600" windowHeight="16380" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alexander1980_alac11" sheetId="1" r:id="rId1"/>
-    <sheet name="auderset-hernandez2020_dura11" sheetId="2" r:id="rId2"/>
-    <sheet name="bradley1970_jica11" sheetId="3" r:id="rId3"/>
-    <sheet name="daly1977_peno11" sheetId="4" r:id="rId4"/>
-    <sheet name="dyk-stoudt1965_gran11" sheetId="5" r:id="rId5"/>
-    <sheet name="farris1992_yoso11" sheetId="6" r:id="rId6"/>
-    <sheet name="good1979_chic12" sheetId="25" r:id="rId7"/>
-    <sheet name="johnson1988_jami11" sheetId="7" r:id="rId8"/>
-    <sheet name="macaulay1996_chal11" sheetId="8" r:id="rId9"/>
-    <sheet name="mak1953_gran11-atat11" sheetId="9" r:id="rId10"/>
-    <sheet name="mak1958_ocot11" sheetId="10" r:id="rId11"/>
-    <sheet name="north-shields1976_prog12" sheetId="11" r:id="rId12"/>
-    <sheet name="overholt1961_metl11" sheetId="12" r:id="rId13"/>
-    <sheet name="pankratz-pike1967_ayut11" sheetId="13" r:id="rId14"/>
-    <sheet name="pensinger1974_jami11" sheetId="14" r:id="rId15"/>
-    <sheet name="pike-cowan1967_huaj11" sheetId="15" r:id="rId16"/>
-    <sheet name="pike-ibach1978_mixt11" sheetId="16" r:id="rId17"/>
-    <sheet name="pike-oram1976_diux11" sheetId="17" r:id="rId18"/>
-    <sheet name="pike-small1974_coat11" sheetId="18" r:id="rId19"/>
-    <sheet name="schultze-jena1938_cahu11" sheetId="19" r:id="rId20"/>
-    <sheet name="shields1988_prog12" sheetId="20" r:id="rId21"/>
-    <sheet name="stark1986_colo11" sheetId="26" r:id="rId22"/>
-    <sheet name="zylstra1980_alac11" sheetId="21" r:id="rId23"/>
-    <sheet name="zylstra1991_alac11" sheetId="22" r:id="rId24"/>
-    <sheet name="durr1987" sheetId="23" r:id="rId25"/>
-    <sheet name="josserand1983" sheetId="24" r:id="rId26"/>
+    <sheet name="amith2020_yolo11" sheetId="27" r:id="rId2"/>
+    <sheet name="auderset-hernandez2020_dura11" sheetId="2" r:id="rId3"/>
+    <sheet name="bradley1970_jica11" sheetId="3" r:id="rId4"/>
+    <sheet name="daly1977_peno11" sheetId="4" r:id="rId5"/>
+    <sheet name="dyk-stoudt1965_gran11" sheetId="5" r:id="rId6"/>
+    <sheet name="farris1992_yoso11" sheetId="6" r:id="rId7"/>
+    <sheet name="good1979_chic12" sheetId="25" r:id="rId8"/>
+    <sheet name="johnson1988_jami11" sheetId="7" r:id="rId9"/>
+    <sheet name="macaulay1996_chal11" sheetId="8" r:id="rId10"/>
+    <sheet name="mak1953_gran11-atat11" sheetId="9" r:id="rId11"/>
+    <sheet name="mak1958_ocot11" sheetId="10" r:id="rId12"/>
+    <sheet name="north-shields1976_prog12" sheetId="11" r:id="rId13"/>
+    <sheet name="overholt1961_metl11" sheetId="12" r:id="rId14"/>
+    <sheet name="pankratz-pike1967_ayut11" sheetId="13" r:id="rId15"/>
+    <sheet name="pensinger1974_jami11" sheetId="14" r:id="rId16"/>
+    <sheet name="pike-cowan1967_huaj11" sheetId="15" r:id="rId17"/>
+    <sheet name="pike-ibach1978_mixt11" sheetId="16" r:id="rId18"/>
+    <sheet name="pike-oram1976_diux11" sheetId="17" r:id="rId19"/>
+    <sheet name="pike-small1974_coat11" sheetId="18" r:id="rId20"/>
+    <sheet name="schultze-jena1938_cahu11" sheetId="19" r:id="rId21"/>
+    <sheet name="shields1988_prog12" sheetId="20" r:id="rId22"/>
+    <sheet name="stark1986_colo11" sheetId="26" r:id="rId23"/>
+    <sheet name="zylstra1980_alac11" sheetId="21" r:id="rId24"/>
+    <sheet name="zylstra1991_alac11" sheetId="22" r:id="rId25"/>
+    <sheet name="durr1987" sheetId="23" r:id="rId26"/>
+    <sheet name="josserand1983" sheetId="24" r:id="rId27"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">alexander1980_alac11!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">bradley1970_jica11!$A$1:$E$53</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">daly1977_peno11!$B$1:$B$168</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'dyk-stoudt1965_gran11'!$B$1:$B$111</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'pike-ibach1978_mixt11'!$A$1:$E$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3">bradley1970_jica11!$A$1:$E$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">daly1977_peno11!$B$1:$B$168</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5">'dyk-stoudt1965_gran11'!$B$1:$B$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'pike-ibach1978_mixt11'!$A$1:$E$39</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5767" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5772" uniqueCount="935">
   <si>
     <t>Grapheme</t>
   </si>
@@ -4579,6 +4580,683 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AMJ57"/>
+  <sheetViews>
+    <sheetView topLeftCell="J1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1024" width="11.5" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMJ39"/>
   <sheetViews>
@@ -5096,7 +5774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
@@ -5532,7 +6210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMJ104"/>
   <sheetViews>
@@ -6792,7 +7470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AMJ51"/>
   <sheetViews>
@@ -7423,7 +8101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
@@ -7905,7 +8583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AMJ109"/>
   <sheetViews>
@@ -9172,7 +9850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
@@ -9613,7 +10291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
@@ -10055,7 +10733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMJ55"/>
   <sheetViews>
@@ -10690,7 +11368,42 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FE69F2F-0474-D14C-A876-C35028168AA3}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMJ67"/>
   <sheetViews>
@@ -12543,1136 +13256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMJ98"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1024" width="11.5" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>847</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>848</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A2:E98">
-    <sortCondition ref="C2:C98"/>
-    <sortCondition ref="B2:B98"/>
-  </sortState>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AMJ39"/>
   <sheetViews>
@@ -14137,7 +13721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
@@ -15250,11 +14834,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BDDB5B-0B55-A64B-84C7-13D4CFC17C1A}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -15285,7 +14869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:AMJ50"/>
   <sheetViews>
@@ -15876,7 +15460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:AMJ97"/>
   <sheetViews>
@@ -16987,7 +16571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:AMJ90"/>
   <sheetViews>
@@ -18441,7 +18025,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:AMJ19"/>
   <sheetViews>
@@ -18663,6 +18247,1135 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMJ98"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1024" width="11.5" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:E98">
+    <sortCondition ref="C2:C98"/>
+    <sortCondition ref="B2:B98"/>
+  </sortState>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ53"/>
   <sheetViews>
@@ -19327,7 +20040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ168"/>
   <sheetViews>
@@ -21223,7 +21936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ111"/>
   <sheetViews>
@@ -22482,7 +23195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ116"/>
   <sheetViews>
@@ -23797,7 +24510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D3DC8BB-3CD1-C443-B76D-FAD255D7212D}">
   <dimension ref="A1:AMJ50"/>
   <sheetViews>
@@ -25522,7 +26235,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ93"/>
   <sheetViews>
@@ -26585,681 +27298,4 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AMJ57"/>
-  <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1024" width="11.5" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>